<commit_message>
finish get basic info
</commit_message>
<xml_diff>
--- a/resources/新建 XLSX 工作表.xlsx
+++ b/resources/新建 XLSX 工作表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9360" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="设计" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="264">
   <si>
     <t>表名</t>
   </si>
@@ -45,75 +45,81 @@
     <t>id</t>
   </si>
   <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>编码规则 国产/进口+药品类型+位顺序编码 （例：0H11）</t>
+  </si>
+  <si>
+    <t>国产：0 进口：1 | H化学药/Z中成药/S生物制品/B保健药品</t>
+  </si>
+  <si>
+    <t>剂型</t>
+  </si>
+  <si>
+    <t>dosageForm</t>
+  </si>
+  <si>
+    <t>批准文号/注册证号</t>
+  </si>
+  <si>
+    <t>approvalNum</t>
+  </si>
+  <si>
+    <t>国产药品使用批准文号，进口药品使用注册证号</t>
+  </si>
+  <si>
+    <t>性状</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>规格</t>
+  </si>
+  <si>
+    <t>specification</t>
+  </si>
+  <si>
+    <t>多值以#隔开</t>
+  </si>
+  <si>
+    <t>处方</t>
+  </si>
+  <si>
+    <t>drugPrescription</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>R/OTC甲类/OTC乙类</t>
+  </si>
+  <si>
+    <t>R:0 OTC甲类：1 OTC乙类：2</t>
+  </si>
+  <si>
+    <t>执行标准</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>有效期</t>
+  </si>
+  <si>
+    <t>validityTerm</t>
+  </si>
+  <si>
+    <t>以月为单位</t>
+  </si>
+  <si>
+    <t>药品名称 name</t>
+  </si>
+  <si>
     <t>char</t>
   </si>
   <si>
-    <t>编码规则 国产/进口+药品类型+位顺序编码 （例：0H0001）</t>
-  </si>
-  <si>
-    <t>国产：0 进口：1 | H化学药/Z中成药/S生物制品/B保健药品 | 顺序编码：十六进制</t>
-  </si>
-  <si>
-    <t>批准文号/注册证号</t>
-  </si>
-  <si>
-    <t>approvalNum</t>
-  </si>
-  <si>
-    <t>varchar</t>
-  </si>
-  <si>
-    <t>国产药品使用批准文号，进口药品使用注册证号</t>
-  </si>
-  <si>
-    <t>性状</t>
-  </si>
-  <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>规格</t>
-  </si>
-  <si>
-    <t>specification</t>
-  </si>
-  <si>
-    <t>多值以#隔开</t>
-  </si>
-  <si>
-    <t>处方</t>
-  </si>
-  <si>
-    <t>drugPrescription</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>R/OTC甲类/OTC乙类</t>
-  </si>
-  <si>
-    <t>R:0 OTC甲类：1 OTC乙类：2</t>
-  </si>
-  <si>
-    <t>执行标准</t>
-  </si>
-  <si>
-    <t>standard</t>
-  </si>
-  <si>
-    <t>有效期</t>
-  </si>
-  <si>
-    <t>validityTerm</t>
-  </si>
-  <si>
-    <t>以月为单位</t>
-  </si>
-  <si>
-    <t>药品名称 name</t>
-  </si>
-  <si>
     <t>通用名称</t>
   </si>
   <si>
@@ -487,6 +493,9 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>片剂</t>
   </si>
   <si>
     <t>name</t>
@@ -811,7 +820,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,6 +839,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -852,8 +869,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -884,45 +940,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -943,9 +961,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -968,21 +985,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -991,13 +1008,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1009,19 +1146,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,157 +1188,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1225,44 +1236,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1293,32 +1292,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1330,10 +1341,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1342,156 +1353,153 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
@@ -1509,13 +1517,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1869,10 +1886,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1885,33 +1902,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1925,180 +1942,178 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="10"/>
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="11"/>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="10"/>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="11"/>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="10"/>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="11"/>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="10"/>
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="11"/>
-      <c r="B7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="10"/>
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="11"/>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="10"/>
+      <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="10" t="s">
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="10"/>
-      <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
@@ -2107,331 +2122,331 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>42</v>
+        <v>7</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="10"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="10"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" ht="13" customHeight="1" spans="1:6">
-      <c r="A19" s="10"/>
+    <row r="19" spans="1:6">
+      <c r="A19" s="9"/>
       <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" ht="13" customHeight="1" spans="1:6">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" ht="13" customHeight="1" spans="1:6">
+      <c r="A21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="10"/>
-      <c r="B21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="10"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="9"/>
+      <c r="B23" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="10" t="s">
+      <c r="C23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="10"/>
-      <c r="B24" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="9"/>
+      <c r="B25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="10"/>
-      <c r="B25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="10"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="3" t="s">
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="9"/>
+      <c r="B27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="10"/>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="9"/>
+      <c r="B28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="10"/>
-      <c r="B28" s="3" t="s">
+      <c r="D28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="F28" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="13" t="s">
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="9"/>
+      <c r="B29" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="10"/>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="10"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="15"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="9"/>
+      <c r="B31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="13"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="10" t="s">
+      <c r="C31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="D31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="15"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="10"/>
-      <c r="B32" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="9"/>
+      <c r="B33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="10"/>
-      <c r="B33" s="14" t="s">
+      <c r="C33" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="9"/>
+      <c r="B34" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="10"/>
-      <c r="B34" s="3" t="s">
+      <c r="D34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>9</v>
@@ -2440,106 +2455,106 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="10"/>
+      <c r="A36" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="B36" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>92</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="10"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="9"/>
+      <c r="B38" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="10" t="s">
+      <c r="D38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="F38" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="10"/>
-      <c r="B39" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="10"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>69</v>
+        <v>100</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>100</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="10"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9"/>
+      <c r="B42" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C42" s="2" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>9</v>
@@ -2548,119 +2563,119 @@
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="10"/>
+      <c r="A43" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="B43" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>105</v>
+        <v>7</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="10"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>107</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="9"/>
+      <c r="B45" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="10"/>
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3" t="s">
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="9"/>
+      <c r="B46" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="10" t="s">
+      <c r="C46" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="D46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="10"/>
-      <c r="B47" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="10"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="C48" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D48" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E48" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="9"/>
+      <c r="B49" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="10"/>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="9"/>
+      <c r="B50" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C50" s="2" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>9</v>
@@ -2669,46 +2684,46 @@
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="10"/>
+      <c r="A51" s="9" t="s">
+        <v>121</v>
+      </c>
       <c r="B51" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>121</v>
+        <v>7</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="9"/>
+      <c r="B52" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="10"/>
-      <c r="B52" s="3" t="s">
+      <c r="D52" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C53" s="2" t="s">
-        <v>8</v>
+        <v>127</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>9</v>
@@ -2717,42 +2732,42 @@
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="10"/>
+      <c r="A54" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="B54" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="10"/>
+      <c r="A55" s="9"/>
       <c r="B55" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>125</v>
+        <v>83</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9"/>
+      <c r="B56" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>9</v>
@@ -2761,28 +2776,28 @@
       <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="10"/>
+      <c r="A57" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="B57" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>129</v>
+        <v>7</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="9"/>
+      <c r="B58" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C58" s="2" t="s">
-        <v>8</v>
+        <v>131</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>9</v>
@@ -2791,42 +2806,42 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="10"/>
+      <c r="A59" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="B59" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>132</v>
+        <v>7</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="10"/>
+      <c r="A60" s="9"/>
       <c r="B60" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>19</v>
+      <c r="C60" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="10" t="s">
-        <v>134</v>
-      </c>
+      <c r="A61" s="9"/>
       <c r="B61" s="3" t="s">
-        <v>7</v>
+        <v>135</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>9</v>
@@ -2835,128 +2850,144 @@
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="10"/>
+      <c r="A62" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="B62" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>136</v>
+        <v>7</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E62" s="3"/>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="9"/>
+      <c r="B63" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="10"/>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="D63" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="10"/>
+      <c r="A64" s="9"/>
       <c r="B64" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>141</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="10"/>
+      <c r="A65" s="9"/>
       <c r="B65" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>143</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="10"/>
+      <c r="A66" s="9"/>
       <c r="B66" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>145</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="10"/>
+      <c r="A67" s="9"/>
       <c r="B67" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="2" t="s">
         <v>147</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="69" ht="15" customHeight="1"/>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
+    <row r="68" spans="1:6">
+      <c r="A68" s="9"/>
+      <c r="B68" s="3" t="s">
         <v>148</v>
       </c>
-    </row>
+      <c r="C68" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="70" ht="15" customHeight="1"/>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="15"/>
+      <c r="A73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="F26:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2969,8 +3000,8 @@
   <sheetPr/>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2986,58 +3017,67 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="D3" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" s="3">
         <v>24</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>157</v>
+      <c r="A5" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3045,38 +3085,41 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>160</v>
-      </c>
+      <c r="D7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>161</v>
+      <c r="A9" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3084,44 +3127,47 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>156</v>
-      </c>
+      <c r="A11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>63</v>
+      <c r="A13" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3129,113 +3175,119 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D15" s="4"/>
+      <c r="A15" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>167</v>
+      <c r="A17" s="4" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>60</v>
+      <c r="B18" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>172</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B20" s="8">
+      <c r="A20" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="7">
         <v>1</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>173</v>
       </c>
+      <c r="F20" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="4"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>174</v>
+      <c r="A22" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3243,135 +3295,139 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>177</v>
+      <c r="A24" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>182</v>
+      <c r="D26" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>185</v>
+      <c r="A27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>187</v>
+      <c r="A28" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>156</v>
+      <c r="A29" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>191</v>
+      <c r="A30" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
+      <c r="A31" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4"/>
       <c r="B32" t="s">
-        <v>195</v>
-      </c>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="4"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>196</v>
+      <c r="A34" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -3379,59 +3435,62 @@
         <v>8</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C36" s="8">
+      <c r="A36" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C36" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C37" s="8">
+      <c r="A37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C38" s="8">
+      <c r="A38" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C39" s="8">
+      <c r="A39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" s="7">
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="4"/>
+    </row>
     <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>201</v>
+      <c r="A41" s="4" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3439,65 +3498,69 @@
         <v>8</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>156</v>
+      <c r="A43" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>156</v>
+      <c r="A44" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
+      <c r="A45" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="4"/>
       <c r="B46" t="s">
-        <v>195</v>
-      </c>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="4"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>207</v>
+      <c r="A48" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3505,65 +3568,69 @@
         <v>8</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>210</v>
+      <c r="A50" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>212</v>
+      <c r="A51" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2">
+      <c r="A52" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="4"/>
       <c r="B53" t="s">
-        <v>195</v>
-      </c>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="4"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>216</v>
+      <c r="A55" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -3571,18 +3638,24 @@
         <v>8</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>118</v>
-      </c>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="4"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>217</v>
+      <c r="A59" s="4" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -3590,48 +3663,51 @@
         <v>8</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B61" s="8">
+      <c r="A61" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="7">
         <v>1</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>218</v>
+      <c r="C61" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B62" s="8">
+      <c r="A62" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B62" s="7">
         <v>0</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>219</v>
+      <c r="C62" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B63" s="8">
+      <c r="A63" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B63" s="7">
         <v>3</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>220</v>
-      </c>
+      <c r="C63" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="4"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" t="s">
-        <v>221</v>
+      <c r="A65" s="4" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -3639,15 +3715,18 @@
         <v>8</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>125</v>
-      </c>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="4"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>222</v>
+      <c r="A68" s="4" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -3655,20 +3734,23 @@
         <v>8</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>223</v>
-      </c>
+      <c r="A70" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="4"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>224</v>
+      <c r="A72" s="4" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -3676,26 +3758,29 @@
         <v>8</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>226</v>
-      </c>
+      <c r="A74" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="4"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>227</v>
+      <c r="A76" s="4" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3703,45 +3788,45 @@
         <v>8</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="D78" s="9">
+      <c r="A78" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D78" s="8">
         <v>210038</v>
       </c>
-      <c r="E78" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>232</v>
+      <c r="E78" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -3764,118 +3849,118 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F4" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D7" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D8" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="4:4">
       <c r="D9" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="4:4">
       <c r="D10" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="4:4">
       <c r="D11" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="4:4">
       <c r="D12" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="4:4">
       <c r="D13" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="4:4">
       <c r="D14" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="4:4">
       <c r="D15" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="4:4">
       <c r="D16" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>